<commit_message>
fix some report's table err
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17655"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="example" sheetId="1" r:id="rId1"/>
@@ -1737,8 +1737,8 @@
   <sheetPr/>
   <dimension ref="A2:AC84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="L57" workbookViewId="0">
-      <selection activeCell="AA71" sqref="AA71"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -5322,7 +5322,7 @@
       <c r="AB67" s="23"/>
       <c r="AC67" s="23"/>
     </row>
-    <row r="68" spans="1:29">
+    <row r="68" ht="15" spans="1:29">
       <c r="A68" s="77"/>
       <c r="B68" s="78"/>
       <c r="C68" s="37"/>
@@ -5369,7 +5369,7 @@
       <c r="AB68" s="23"/>
       <c r="AC68" s="23"/>
     </row>
-    <row r="69" spans="1:29">
+    <row r="69" ht="15" spans="1:29">
       <c r="A69" s="80" t="s">
         <v>67</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>21</v>
       </c>
       <c r="D69" s="83">
-        <v>52111407.1191667</v>
+        <v>35127792.6561062</v>
       </c>
       <c r="E69" s="83">
         <f>SUM(E70:E72)</f>
@@ -5389,11 +5389,11 @@
       </c>
       <c r="G69" s="83">
         <f>E69-D69</f>
-        <v>4369520.3208333</v>
+        <v>21353134.7838938</v>
       </c>
       <c r="H69" s="84">
         <f t="shared" ref="H69:H74" si="10">E69/D69</f>
-        <v>1.08384959382964</v>
+        <v>1.6078700985552</v>
       </c>
       <c r="I69" s="83">
         <f>E69-F69</f>
@@ -5408,6 +5408,7 @@
         <v>52111407.1191666</v>
       </c>
       <c r="L69" s="83">
+        <f>SUM(L70:L72)</f>
         <v>56480927.44</v>
       </c>
       <c r="M69" s="83">
@@ -5418,7 +5419,7 @@
         <v>4369520.3208334</v>
       </c>
       <c r="O69" s="84">
-        <f>L69/K69</f>
+        <f>IF(K69&lt;&gt;0,L69/K69,"-")</f>
         <v>1.08384959382965</v>
       </c>
       <c r="P69" s="83">
@@ -5426,7 +5427,7 @@
         <v>24683375.57</v>
       </c>
       <c r="Q69" s="84">
-        <f>L69/M69</f>
+        <f>IF(M69&lt;&gt;0,L69/M69,"-")</f>
         <v>1.77626653998127</v>
       </c>
       <c r="R69" s="23"/>
@@ -5442,7 +5443,7 @@
       <c r="AB69" s="23"/>
       <c r="AC69" s="23"/>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" ht="15" spans="1:29">
       <c r="A70" s="80" t="s">
         <v>29</v>
       </c>
@@ -5451,7 +5452,7 @@
         <v>21</v>
       </c>
       <c r="D70" s="85">
-        <v>19119614.3333333</v>
+        <v>10876005</v>
       </c>
       <c r="E70" s="85">
         <v>20168229.13</v>
@@ -5465,7 +5466,7 @@
       </c>
       <c r="H70" s="86">
         <f t="shared" si="10"/>
-        <v>1.05484497638839</v>
+        <v>1.85437843491245</v>
       </c>
       <c r="I70" s="85">
         <f>E70-F70</f>
@@ -5489,7 +5490,7 @@
         <v>1048614.7966667</v>
       </c>
       <c r="O70" s="86">
-        <f t="shared" ref="O70:O81" si="13">L70/K70</f>
+        <f t="shared" ref="O70:O81" si="13">IF(K70&lt;&gt;0,L70/K70,"-")</f>
         <v>1.05484497638839</v>
       </c>
       <c r="P70" s="85">
@@ -5497,7 +5498,7 @@
         <v>-1526488.7</v>
       </c>
       <c r="Q70" s="86">
-        <f t="shared" ref="Q70:Q81" si="15">L70/M70</f>
+        <f t="shared" ref="Q70:Q81" si="15">IF(M70&lt;&gt;0,L70/M70,"-")</f>
         <v>0.929637771186444</v>
       </c>
       <c r="R70" s="23"/>
@@ -5513,7 +5514,7 @@
       <c r="AB70" s="23"/>
       <c r="AC70" s="23"/>
     </row>
-    <row r="71" spans="1:29">
+    <row r="71" ht="15" spans="1:29">
       <c r="A71" s="80" t="s">
         <v>68</v>
       </c>
@@ -5522,7 +5523,7 @@
         <v>21</v>
       </c>
       <c r="D71" s="85">
-        <v>32032821.3333333</v>
+        <v>23426769.8761062</v>
       </c>
       <c r="E71" s="85">
         <v>35329356.39</v>
@@ -5532,11 +5533,11 @@
       </c>
       <c r="G71" s="85">
         <f>E71-D71</f>
-        <v>3296535.0566667</v>
+        <v>11902586.5138938</v>
       </c>
       <c r="H71" s="86">
         <f t="shared" si="10"/>
-        <v>1.10291116796622</v>
+        <v>1.50807629804883</v>
       </c>
       <c r="I71" s="85">
         <f t="shared" ref="I71:I81" si="16">E71-F71</f>
@@ -5593,7 +5594,7 @@
         <v>21</v>
       </c>
       <c r="D72" s="85">
-        <v>958971.4525</v>
+        <v>825017.78</v>
       </c>
       <c r="E72" s="85">
         <v>983341.92</v>
@@ -5603,11 +5604,11 @@
       </c>
       <c r="G72" s="85">
         <f>E72-D72</f>
-        <v>24370.4675</v>
+        <v>158324.14</v>
       </c>
       <c r="H72" s="86">
         <f t="shared" si="10"/>
-        <v>1.02541313136743</v>
+        <v>1.19190391266477</v>
       </c>
       <c r="I72" s="85">
         <f t="shared" si="16"/>
@@ -5654,7 +5655,7 @@
       <c r="AB72" s="23"/>
       <c r="AC72" s="23"/>
     </row>
-    <row r="73" spans="1:29">
+    <row r="73" ht="15" spans="1:29">
       <c r="A73" s="80" t="s">
         <v>70</v>
       </c>
@@ -5663,7 +5664,7 @@
         <v>21</v>
       </c>
       <c r="D73" s="83">
-        <v>50908946.4396988</v>
+        <v>34621177.9939547</v>
       </c>
       <c r="E73" s="83">
         <f>SUM(E74:E79)</f>
@@ -5674,11 +5675,11 @@
       </c>
       <c r="G73" s="83">
         <f>E73-D73</f>
-        <v>2290069.5803012</v>
+        <v>18577838.0260453</v>
       </c>
       <c r="H73" s="84">
         <f t="shared" si="10"/>
-        <v>1.04498363726725</v>
+        <v>1.53660329031234</v>
       </c>
       <c r="I73" s="83">
         <f t="shared" si="16"/>
@@ -5693,6 +5694,7 @@
         <v>50908946.4396988</v>
       </c>
       <c r="L73" s="83">
+        <f>SUM(L74:L79)</f>
         <v>53199016.02</v>
       </c>
       <c r="M73" s="83">
@@ -5700,7 +5702,7 @@
       </c>
       <c r="N73" s="83">
         <f t="shared" si="12"/>
-        <v>2290069.58030122</v>
+        <v>2290069.5803012</v>
       </c>
       <c r="O73" s="84">
         <f t="shared" si="13"/>
@@ -5727,7 +5729,7 @@
       <c r="AB73" s="23"/>
       <c r="AC73" s="23"/>
     </row>
-    <row r="74" spans="1:29">
+    <row r="74" ht="15" spans="1:29">
       <c r="A74" s="80" t="s">
         <v>71</v>
       </c>
@@ -5736,7 +5738,7 @@
         <v>21</v>
       </c>
       <c r="D74" s="85">
-        <v>47766210.3715097</v>
+        <v>33183618.0825148</v>
       </c>
       <c r="E74" s="85">
         <v>50259080.46</v>
@@ -5746,11 +5748,11 @@
       </c>
       <c r="G74" s="85">
         <f>E74-D74</f>
-        <v>2492870.0884903</v>
+        <v>17075462.3774852</v>
       </c>
       <c r="H74" s="86">
         <f t="shared" si="10"/>
-        <v>1.05218898608664</v>
+        <v>1.51457506336485</v>
       </c>
       <c r="I74" s="85">
         <f t="shared" si="16"/>
@@ -5807,7 +5809,7 @@
         <v>21</v>
       </c>
       <c r="D75" s="85">
-        <v>319.07375</v>
+        <v>981.006666666667</v>
       </c>
       <c r="E75" s="85">
         <v>0</v>
@@ -5817,7 +5819,7 @@
       </c>
       <c r="G75" s="85">
         <f t="shared" ref="G75:G81" si="17">E75-D75</f>
-        <v>-319.07375</v>
+        <v>-981.006666666667</v>
       </c>
       <c r="H75" s="86">
         <f t="shared" ref="H75:H81" si="18">E75/D75</f>
@@ -5878,7 +5880,7 @@
         <v>21</v>
       </c>
       <c r="D76" s="85">
-        <v>2652406.54900391</v>
+        <v>1051656.26224918</v>
       </c>
       <c r="E76" s="85">
         <v>2328769.95</v>
@@ -5888,11 +5890,11 @@
       </c>
       <c r="G76" s="85">
         <f t="shared" si="17"/>
-        <v>-323636.59900391</v>
+        <v>1277113.68775082</v>
       </c>
       <c r="H76" s="86">
         <f t="shared" si="18"/>
-        <v>0.877983788297669</v>
+        <v>2.2143831911574</v>
       </c>
       <c r="I76" s="85">
         <f t="shared" si="16"/>
@@ -5949,7 +5951,7 @@
         <v>21</v>
       </c>
       <c r="D77" s="85">
-        <v>244630.125333333</v>
+        <v>245218.265555556</v>
       </c>
       <c r="E77" s="85">
         <v>362655.48</v>
@@ -5959,11 +5961,11 @@
       </c>
       <c r="G77" s="85">
         <f t="shared" si="17"/>
-        <v>118025.354666667</v>
+        <v>117437.214444444</v>
       </c>
       <c r="H77" s="86">
         <f t="shared" si="18"/>
-        <v>1.48246451456396</v>
+        <v>1.47890891887023</v>
       </c>
       <c r="I77" s="85">
         <f t="shared" si="16"/>
@@ -6020,7 +6022,7 @@
         <v>21</v>
       </c>
       <c r="D78" s="85">
-        <v>103350.23065</v>
+        <v>108177.162801852</v>
       </c>
       <c r="E78" s="85">
         <v>64840.6800000001</v>
@@ -6030,11 +6032,11 @@
       </c>
       <c r="G78" s="85">
         <f t="shared" si="17"/>
-        <v>-38509.5506499999</v>
+        <v>-43336.4828018519</v>
       </c>
       <c r="H78" s="86">
         <f t="shared" si="18"/>
-        <v>0.627387859632223</v>
+        <v>0.599393423903793</v>
       </c>
       <c r="I78" s="85">
         <f t="shared" si="16"/>
@@ -6091,7 +6093,7 @@
         <v>21</v>
       </c>
       <c r="D79" s="85">
-        <v>142030.089451852</v>
+        <v>31527.2141666667</v>
       </c>
       <c r="E79" s="85">
         <v>183669.45</v>
@@ -6101,11 +6103,11 @@
       </c>
       <c r="G79" s="85">
         <f t="shared" si="17"/>
-        <v>41639.360548148</v>
+        <v>152142.235833333</v>
       </c>
       <c r="H79" s="86">
         <f t="shared" si="18"/>
-        <v>1.29317281083783</v>
+        <v>5.82574308751299</v>
       </c>
       <c r="I79" s="85">
         <f t="shared" si="16"/>
@@ -6162,7 +6164,7 @@
         <v>21</v>
       </c>
       <c r="D80" s="85">
-        <v>-30660.4557979019</v>
+        <v>-15418.4689269971</v>
       </c>
       <c r="E80" s="85">
         <v>426110.93</v>
@@ -6172,11 +6174,11 @@
       </c>
       <c r="G80" s="85">
         <f t="shared" si="17"/>
-        <v>456771.385797902</v>
+        <v>441529.398926997</v>
       </c>
       <c r="H80" s="86">
         <f t="shared" si="18"/>
-        <v>-13.8977363157517</v>
+        <v>-27.6363971038588</v>
       </c>
       <c r="I80" s="85">
         <f t="shared" si="16"/>
@@ -6233,9 +6235,10 @@
         <v>21</v>
       </c>
       <c r="D81" s="83">
-        <v>1171800.22366995</v>
+        <v>491196.193224533</v>
       </c>
       <c r="E81" s="83">
+        <f>E69-E73+E80</f>
         <v>3708022.34999999</v>
       </c>
       <c r="F81" s="83">
@@ -6243,11 +6246,11 @@
       </c>
       <c r="G81" s="83">
         <f t="shared" si="17"/>
-        <v>2536222.12633004</v>
+        <v>3216826.15677546</v>
       </c>
       <c r="H81" s="84">
         <f t="shared" si="18"/>
-        <v>3.1643809884136</v>
+        <v>7.54896393976124</v>
       </c>
       <c r="I81" s="83">
         <f t="shared" si="16"/>

</xml_diff>